<commit_message>
Removed non-ASCII characters from raw data
</commit_message>
<xml_diff>
--- a/data-raw/ve_outcome_lookup.xlsx
+++ b/data-raw/ve_outcome_lookup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelabers/Desktop/VIP/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0564D39C-3967-FD4E-B803-9A2079D10645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE54C594-F549-F744-AE36-B45B625A60A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="26240" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -426,9 +426,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +725,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
@@ -1479,7 +1476,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
+      <c r="A63" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C104" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>